<commit_message>
Series de tiempo, raíz unitaria y cointegración
</commit_message>
<xml_diff>
--- a/Proyecto Interno/Precios al por mayor/Mapeo SIPSA-TCAC/1823_mapeo_sipsa_tcac.xlsx
+++ b/Proyecto Interno/Precios al por mayor/Mapeo SIPSA-TCAC/1823_mapeo_sipsa_tcac.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B366"/>
+  <dimension ref="A1:B384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1307,87 +1307,82 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Cebolla cabezona blanca importada</t>
+          <t>Cebolla cabezona blanca ecuatoriana</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Cebolla cabezona blanca pastusa</t>
+          <t>Cebolla cabezona blanca importada</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Cebolla cabezona roja</t>
+          <t>Cebolla cabezona blanca pastusa</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Cebolla cabezona roja importada</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>B027</t>
+          <t>Cebolla cabezona blanca peruana</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Cebolla cabezona roja ocañera</t>
+          <t>Cebolla cabezona roja</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Cebolla cabezona roja peruana</t>
+          <t>Cebolla cabezona roja ecuatoriana</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Cebolla junca</t>
+          <t>Cebolla cabezona roja importada</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>B027</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Cebolla junca Aquitania</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>B029</t>
+          <t>Cebolla cabezona roja ocañera</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Cebolla junca Berlín</t>
+          <t>Cebolla cabezona roja peruana</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Cebolla junca pastusa</t>
+          <t>Cebolla junca</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Cebolla junca Tenerife</t>
+          <t>Cebolla junca Aquitania</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1399,2291 +1394,2422 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Cebolla puerro</t>
+          <t>Cebolla junca Berlín</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Cebollín chino</t>
+          <t>Cebolla junca pastusa</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Chocolate amargo</t>
+          <t>Cebolla junca Tenerife</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>L008</t>
+          <t>B029</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Chocolate dulce</t>
+          <t>Cebolla puerro</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Chocolate instantáneo</t>
+          <t>Cebollín chino</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Chócolo mazorca</t>
+          <t>Chocolate amargo</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>A053</t>
+          <t>L008</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Cidra</t>
+          <t>Chocolate dulce</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Cilantro</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>EX000</t>
+          <t>Chocolate instantáneo</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Ciruela importada</t>
+          <t>Chócolo mazorca</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>A053</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Ciruela roja</t>
+          <t>Cidra</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Coco</t>
+          <t>Cilantro</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>C019</t>
+          <t>EX000</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Coles</t>
+          <t>Ciruela importada</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Coliflor</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>B039</t>
+          <t>Ciruela negra chilena</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Color (bolsita)</t>
+          <t>Ciruela negra importada</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Corvina, filete congelado nacional</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>E021</t>
+          <t>Ciruela roja</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Cuchuco de cebada</t>
+          <t>Coco</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>C019</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Cuchuco de maíz</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>A044</t>
+          <t>Coles</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Curuba</t>
+          <t>Coliflor</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>C021</t>
+          <t>B039</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Durazno importado</t>
+          <t>Color (bolsita)</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Durazno nacional</t>
+          <t>Corvina, filete congelado nacional</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>E021</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Espinaca</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>B044</t>
+          <t>Cuchuco de cebada</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Fécula de maíz</t>
+          <t>Cuchuco de maíz</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>A044</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Feijoa</t>
+          <t>Curuba</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>C021</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Fresa</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>C025</t>
+          <t>Curuba redonda</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Fríjol bolón</t>
+          <t>Durazno importado</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Fríjol cabeza negra importado</t>
+          <t>Durazno nacional</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Fríjol cabeza negra nacional</t>
+          <t>Espinaca</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>B044</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Fríjol calima</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>T015</t>
+          <t>Fécula de maíz</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Fríjol cargamanto blanco</t>
+          <t>Feijoa</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Fríjol cargamanto rojo</t>
+          <t>Fresa</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>C025</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Fríjol enlatado</t>
+          <t>Fríjol bolón</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Fríjol nima calima</t>
+          <t>Fríjol cabeza negra importado</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Fríjol palomito importado</t>
+          <t>Fríjol cabeza negra nacional</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Fríjol radical</t>
+          <t>Fríjol calima</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>T015</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Fríjol Uribe rosado</t>
+          <t>Fríjol cargamanto blanco</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Fríjol verde bolo</t>
+          <t>Fríjol cargamanto rojo</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Fríjol verde cargamanto</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>B046</t>
+          <t>Fríjol enlatado</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Fríjol verde en vaina</t>
+          <t>Fríjol nima calima</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Fríjol Zaragoza</t>
+          <t>Fríjol palomito importado</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Galletas dulces redondas con crema</t>
+          <t>Fríjol radical</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Galletas saladas</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>A027</t>
+          <t>Fríjol Uribe rosado</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Garbanzo importado</t>
+          <t>Fríjol verde bolo</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Gelatina</t>
+          <t>Fríjol verde cargamanto</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>K018</t>
+          <t>B046</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Granadilla</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>C028</t>
+          <t>Fríjol verde en vaina</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Guanábana</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>C030</t>
+          <t>Fríjol Zaragoza</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Guayaba agria</t>
+          <t>Galletas dulces redondas con crema</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Guayaba Atlántico</t>
+          <t>Galletas saladas</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>A027</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Guayaba común</t>
+          <t>Galletas saladas 3 tacos</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Guayaba manzana</t>
+          <t>Garbanzo importado</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Guayaba pera</t>
+          <t>Gelatina</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>C032</t>
+          <t>K018</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Guayaba pera valluna</t>
+          <t>Granadilla</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>C028</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Gulupa</t>
+          <t>Guanábana</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>C030</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Haba verde</t>
+          <t>Guayaba agria</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Habichuela</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>B052</t>
+          <t>Guayaba Atlántico</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Habichuela larga</t>
+          <t>Guayaba común</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Harina de trigo</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>A040</t>
+          <t>Guayaba manzana</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Harina precocida de maíz</t>
+          <t>Guayaba pera</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>A034</t>
+          <t>C032</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Higo</t>
+          <t>Guayaba pera valluna</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Huevo blanco A</t>
+          <t>Gulupa</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Huevo blanco AA</t>
+          <t>Haba verde</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Huevo blanco B</t>
+          <t>Habichuela</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>B052</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Huevo blanco extra</t>
+          <t>Habichuela larga</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Huevo rojo A</t>
+          <t>Harina de trigo</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>J004</t>
+          <t>A040</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Huevo rojo AA</t>
+          <t>Harina precocida de maíz</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>J004</t>
+          <t>A034</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Huevo rojo B</t>
+          <t>Higo</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Huevo rojo extra</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>J004</t>
+          <t>Huevo blanco A</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Jugo de frutas</t>
+          <t>Huevo blanco AA</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Jugo instantáneo (sobre)</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>K018</t>
+          <t>Huevo blanco B</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Kiwi</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>C042</t>
+          <t>Huevo blanco extra</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Langostino 16-20</t>
+          <t>Huevo rojo A</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>E024</t>
+          <t>J004</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Langostino U12</t>
+          <t>Huevo rojo AA</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>E024</t>
+          <t>J004</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Leche en polvo</t>
-        </is>
-      </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>G008</t>
+          <t>Huevo rojo B</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Lechuga Batavia</t>
+          <t>Huevo rojo extra</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>B059</t>
+          <t>J004</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Lechuga crespa verde</t>
-        </is>
-      </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>B060</t>
+          <t>Jugo de frutas</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Lenteja importada</t>
+          <t>Jugo instantáneo (sobre)</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>T026</t>
+          <t>K018</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Limón común</t>
+          <t>Kiwi</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>C044</t>
+          <t>C042</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Limón común Ciénaga</t>
+          <t>Langostino 16-20</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>E024</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Limón común valluno</t>
+          <t>Langostino U12</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>E024</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Limón mandarino</t>
+          <t>Leche en polvo</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>C044</t>
+          <t>G008</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Limón Tahití</t>
+          <t>Lechuga Batavia</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>C044</t>
+          <t>B059</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Lomitos de atún en lata</t>
-        </is>
-      </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>E003</t>
+          <t>Lechuga crespa morada</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Lulo</t>
+          <t>Lechuga crespa verde</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>C045</t>
+          <t>B060</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Maíz amarillo cáscara</t>
+          <t>Lenteja importada</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>T026</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Maíz amarillo cáscara importado</t>
+          <t>Lenteja nacional</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Maíz amarillo trillado</t>
+          <t>Limón común</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>A044</t>
+          <t>C044</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Maíz blanco cáscara</t>
+          <t>Limón común Ciénaga</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Maíz blanco retrillado</t>
+          <t>Limón común ecuatoriano</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Maíz blanco trillado</t>
-        </is>
-      </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>A046</t>
+          <t>Limón común valluno</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Maíz enlatado</t>
+          <t>Limón mandarino</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>C044</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Maíz pira</t>
+          <t>Limón Tahití</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>C044</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Mandarina arrayana</t>
+          <t>Lomitos de atún en lata</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>E003</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Mandarina Arrayana</t>
+          <t>Lulo</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>C050</t>
+          <t>C045</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Mandarina común</t>
+          <t>Maíz amarillo cáscara</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Mandarina Oneco</t>
-        </is>
-      </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>C050</t>
+          <t>Maíz amarillo cáscara importado</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Mango común</t>
-        </is>
-      </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>C051</t>
+          <t>Maíz amarillo retrillado</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Mango costeño</t>
+          <t>Maíz amarillo trillado</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>A044</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Mango de azúcar</t>
+          <t>Maíz blanco cáscara</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Mango Kent</t>
+          <t>Maíz blanco retrillado</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Mango manzano</t>
+          <t>Maíz blanco trillado</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>A046</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Mango reina</t>
+          <t>Maíz enlatado</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Mango Tommy</t>
-        </is>
-      </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>C052</t>
+          <t>Maíz pira</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Mango Yulima</t>
+          <t>Mandarina arrayana</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Manteca</t>
+          <t>Mandarina Arrayana</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>C050</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Manzana nacional</t>
+          <t>Mandarina común</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Manzana roja importada</t>
+          <t>Mandarina Oneco</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>C054</t>
+          <t>C050</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Manzana royal gala importada</t>
+          <t>Mango común</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>C054</t>
+          <t>C051</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Manzana verde importada</t>
-        </is>
-      </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>C054</t>
+          <t>Mango costeño</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Maracuyá</t>
-        </is>
-      </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>C056</t>
+          <t>Mango de azúcar</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Maracuyá antioqueño</t>
+          <t>Mango Kent</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Maracuyá huilense</t>
+          <t>Mango manzano</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Maracuyá santandereano</t>
+          <t>Mango mariquiteño</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Maracuyá valluno</t>
+          <t>Mango reina</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Margarina</t>
+          <t>Mango Tommy</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>D018</t>
+          <t>C052</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Mayonesa doy pack</t>
-        </is>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>D020</t>
+          <t>Mango Yulima</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Melón Cantalup</t>
-        </is>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>C060</t>
+          <t>Manteca</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Menudencias de pollo</t>
+          <t>Manzana nacional</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Merluza, filete importado</t>
+          <t>Manzana roja importada</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>E030</t>
+          <t>C054</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Merluza, filete nacional</t>
+          <t>Manzana royal gala importada</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>E030</t>
+          <t>C054</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Mojarra lora entera congelada</t>
+          <t>Manzana verde importada</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>C054</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Mojarra lora entera fresca</t>
+          <t>Maracuyá</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>C056</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Mora de Castilla</t>
-        </is>
-      </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>C061</t>
+          <t>Maracuyá antioqueño</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Mostaza doy pack</t>
+          <t>Maracuyá huilense</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Muslos de pollo con rabadilla</t>
+          <t>Maracuyá santandereano</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Muslos de pollo sin rabadilla</t>
+          <t>Maracuyá valluno</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Naranja común</t>
+          <t>Margarina</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>D018</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Naranja Sweet</t>
+          <t>Mayonesa doy pack</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>C062</t>
+          <t>D020</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Naranja Valencia</t>
+          <t>Melón Cantalup</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>C060</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Nicuro fresco</t>
+          <t>Menudencias de pollo</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Ñame criollo</t>
+          <t>Merluza, filete importado</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>E030</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Ñame diamante</t>
+          <t>Merluza, filete nacional</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>E030</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Ñame espino</t>
+          <t>Mojarra lora entera congelada</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Palmitos de mar</t>
+          <t>Mojarra lora entera fresca</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Panela cuadrada blanca</t>
+          <t>Mora de Castilla</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>C061</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Panela cuadrada morena</t>
+          <t>Mostaza doy pack</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Panela en pastilla</t>
+          <t>Muslos de pollo con rabadilla</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Panela redonda blanca</t>
+          <t>Muslos de pollo sin rabadilla</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Panela redonda morena</t>
-        </is>
-      </c>
-      <c r="B249" t="inlineStr">
-        <is>
-          <t>K033</t>
+          <t>Naranja común</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Papa Betina</t>
+          <t>Naranja Sweet</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>B074</t>
+          <t>C062</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Papa capira</t>
-        </is>
-      </c>
-      <c r="B251" t="inlineStr">
-        <is>
-          <t>B074</t>
+          <t>Naranja Valencia</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Papa criolla limpia</t>
-        </is>
-      </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>B071</t>
+          <t>Nicuro fresco</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Papa criolla sucia</t>
-        </is>
-      </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>B071</t>
+          <t>Ñame criollo</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Papa ICA-Huila</t>
+          <t>Ñame diamante</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Papa Morasurco</t>
+          <t>Ñame espino</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Papa nevada</t>
+          <t>Palmitos de mar</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Papa parda pastusa</t>
-        </is>
-      </c>
-      <c r="B257" t="inlineStr">
-        <is>
-          <t>B074</t>
+          <t>Panela cuadrada blanca</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Papa Puracé</t>
+          <t>Panela cuadrada morena</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Papa R-12 negra</t>
+          <t>Panela en pastilla</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Papa R-12 roja</t>
+          <t>Panela redonda blanca</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Papa roja peruana</t>
+          <t>Panela redonda morena</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>K033</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Papa rubí</t>
+          <t>Papa Betina</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>B074</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Papa sabanera</t>
+          <t>Papa capira</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>B074</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Papa San Félix</t>
+          <t>Papa criolla limpia</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>B071</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Papa superior</t>
+          <t>Papa criolla para lavar</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Papa suprema</t>
+          <t>Papa criolla sucia</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>B074</t>
+          <t>B071</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Papa tocarreña</t>
+          <t>Papa frita</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Papa única</t>
-        </is>
-      </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>B074</t>
+          <t>Papa ICA-Huila</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Papaya hawaiana</t>
+          <t>Papa Morasurco</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Papaya Maradol</t>
-        </is>
-      </c>
-      <c r="B270" t="inlineStr">
-        <is>
-          <t>C065</t>
+          <t>Papa nevada</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Papaya melona</t>
+          <t>Papa parda pastusa</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>B074</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Papaya Paulina</t>
+          <t>Papa Puracé</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Papaya redonda</t>
+          <t>Papa R-12 negra</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Papaya tainung</t>
+          <t>Papa R-12 roja</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Pargo rojo entero congelado</t>
-        </is>
-      </c>
-      <c r="B275" t="inlineStr">
-        <is>
-          <t>E043</t>
+          <t>Papa roja peruana</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Pargo rojo entero fresco</t>
+          <t>Papa rubí</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Pargo rojo platero</t>
+          <t>Papa sabanera</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Pastas alimenticias</t>
-        </is>
-      </c>
-      <c r="B278" t="inlineStr">
-        <is>
-          <t>A072</t>
+          <t>Papa San Félix</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Patilla</t>
-        </is>
-      </c>
-      <c r="B279" t="inlineStr">
-        <is>
-          <t>C079</t>
+          <t>Papa superior</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Patilla baby</t>
+          <t>Papa suprema</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>C079</t>
+          <t>B074</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Pechuga de pollo</t>
-        </is>
-      </c>
-      <c r="B281" t="inlineStr">
-        <is>
-          <t>F085</t>
+          <t>Papa tocana</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Pepino cohombro</t>
-        </is>
-      </c>
-      <c r="B282" t="inlineStr">
-        <is>
-          <t>B077</t>
+          <t>Papa tocarreña</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Pepino de rellenar</t>
+          <t>Papa única</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>B074</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Pera importada</t>
-        </is>
-      </c>
-      <c r="B284" t="inlineStr">
-        <is>
-          <t>C071</t>
+          <t>Papaya hawaiana</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Pera nacional</t>
+          <t>Papaya Maradol</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>C065</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Perejil</t>
+          <t>Papaya melona</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Pescado cabezas</t>
-        </is>
-      </c>
-      <c r="B287" t="inlineStr">
-        <is>
-          <t>E002</t>
+          <t>Papaya Paulina</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Pierna pernil con rabadilla</t>
-        </is>
-      </c>
-      <c r="B288" t="inlineStr">
-        <is>
-          <t>F091</t>
+          <t>Papaya redonda</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Pierna pernil sin rabadilla</t>
+          <t>Papaya tainung</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Piernas de pollo</t>
+          <t>Pargo rojo entero congelado</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>F091</t>
+          <t>E043</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Pimentón</t>
-        </is>
-      </c>
-      <c r="B291" t="inlineStr">
-        <is>
-          <t>B080</t>
+          <t>Pargo rojo entero fresco</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Pimentón verde</t>
+          <t>Pargo rojo platero</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Piña gold</t>
+          <t>Pastas alimenticias</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>C072</t>
+          <t>A072</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Piña manzana</t>
+          <t>Patilla</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>C072</t>
+          <t>C079</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Piña perolera</t>
+          <t>Patilla baby</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>C079</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Pitahaya</t>
+          <t>Pechuga de pollo</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>F085</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Plátano comino</t>
+          <t>Pepino cohombro</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>B077</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Plátano dominico hartón maduro</t>
+          <t>Pepino de rellenar</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Plátano dominico hartón verde</t>
+          <t>Pera importada</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>C071</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Plátano dominico verde</t>
+          <t>Pera nacional</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Plátano guineo</t>
+          <t>Perejil</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Plátano hartón maduro</t>
+          <t>Pescado cabezas</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>E002</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Plátano hartón verde</t>
+          <t>Pierna pernil con rabadilla</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>B092</t>
+          <t>F091</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Plátano hartón verde ecuatoriano</t>
+          <t>Pierna pernil sin rabadilla</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Plátano hartón verde Eje Cafetero</t>
+          <t>Piernas de pollo</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>F091</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Plátano hartón verde llanero</t>
+          <t>Pimentón</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>B080</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Pollo entero congelado sin vísceras</t>
-        </is>
-      </c>
-      <c r="B307" t="inlineStr">
-        <is>
-          <t>F077</t>
+          <t>Pimentón verde</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>Pollo entero fresco con vísceras</t>
+          <t>Piña Cayena</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Pollo entero fresco sin vísceras</t>
+          <t>Piña gold</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>C072</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Queso campesino</t>
+          <t>Piña manzana</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>G017</t>
+          <t>C072</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Queso Caquetá</t>
-        </is>
-      </c>
-      <c r="B311" t="inlineStr">
-        <is>
-          <t>G020</t>
+          <t>Piña perolera</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Queso costeño</t>
-        </is>
-      </c>
-      <c r="B312" t="inlineStr">
-        <is>
-          <t>G018</t>
+          <t>Pitahaya</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Queso cuajada</t>
-        </is>
-      </c>
-      <c r="B313" t="inlineStr">
-        <is>
-          <t>G016</t>
+          <t>Plátano comino</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Queso doble crema</t>
-        </is>
-      </c>
-      <c r="B314" t="inlineStr">
-        <is>
-          <t>G021</t>
+          <t>Plátano dominico hartón maduro</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Rabadillas de pollo</t>
+          <t>Plátano dominico hartón verde</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Rábano rojo</t>
+          <t>Plátano dominico verde</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Remolacha</t>
+          <t>Plátano guineo</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Remolacha bogotana</t>
-        </is>
-      </c>
-      <c r="B318" t="inlineStr">
-        <is>
-          <t>B098</t>
+          <t>Plátano hartón maduro</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Remolacha regional</t>
+          <t>Plátano hartón verde</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>B092</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Repollo blanco</t>
-        </is>
-      </c>
-      <c r="B320" t="inlineStr">
-        <is>
-          <t>B099</t>
+          <t>Plátano hartón verde ecuatoriano</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Repollo blanco bogotano</t>
+          <t>Plátano hartón verde Eje Cafetero</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Repollo blanco valluno</t>
+          <t>Plátano hartón verde llanero</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>Repollo morado</t>
+          <t>Plátano hartón verde venezolano</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Repollo verde</t>
+          <t>Pollo entero congelado con vísceras</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>Róbalo, filete congelado</t>
+          <t>Pollo entero congelado sin vísceras</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>F077</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>Sal yodada</t>
-        </is>
-      </c>
-      <c r="B326" t="inlineStr">
-        <is>
-          <t>L015</t>
+          <t>Pollo entero fresco con vísceras</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>Salmón, filete congelado</t>
-        </is>
-      </c>
-      <c r="B327" t="inlineStr">
-        <is>
-          <t>E038</t>
+          <t>Pollo entero fresco sin vísceras</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>Salsa de tomate doy pack</t>
+          <t>Queso campesino</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>L017</t>
+          <t>G017</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Sardinas en lata</t>
+          <t>Queso Caquetá</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>E039</t>
+          <t>G020</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>Sierra entera congelada</t>
+          <t>Queso costeño</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>E041</t>
+          <t>G018</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>Sopa de pollo (caja)</t>
+          <t>Queso cuajada</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>G016</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>Tangelo</t>
+          <t>Queso doble crema</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>G021</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Tilapia roja entera congelada</t>
-        </is>
-      </c>
-      <c r="B333" t="inlineStr">
-        <is>
-          <t>E043</t>
+          <t>Rabadillas de pollo</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Tilapia roja entera fresca</t>
+          <t>Rábano rojo</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Tilapia, filete congelado</t>
-        </is>
-      </c>
-      <c r="B335" t="inlineStr">
-        <is>
-          <t>E030</t>
+          <t>Remolacha</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Tilapia, lomitos</t>
+          <t>Remolacha bogotana</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>B098</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Tomate chonto</t>
-        </is>
-      </c>
-      <c r="B337" t="inlineStr">
-        <is>
-          <t>B103</t>
+          <t>Remolacha regional</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Tomate chonto regional</t>
+          <t>Repollo blanco</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>B099</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Tomate chonto valluno</t>
+          <t>Repollo blanco bogotano</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Tomate de árbol</t>
-        </is>
-      </c>
-      <c r="B340" t="inlineStr">
-        <is>
-          <t>C082</t>
+          <t>Repollo blanco valluno</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Tomate larga vida</t>
-        </is>
-      </c>
-      <c r="B341" t="inlineStr">
-        <is>
-          <t>B103</t>
+          <t>Repollo morado</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Tomate riñón</t>
+          <t>Repollo verde</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Tomate riñón valluno</t>
+          <t>Róbalo, filete congelado</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Tomate Riogrande</t>
+          <t>Sal yodada</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>L015</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Tomate Riogrande bumangués</t>
+          <t>Salmón, filete congelado</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>E038</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Tomate Riogrande ocañero</t>
+          <t>Salsa de tomate doy pack</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>L017</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Toyo blanco, filete congelado</t>
+          <t>Sardinas en lata</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>E039</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Trucha en corte mariposa</t>
+          <t>Sierra entera congelada</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>E047</t>
+          <t>E041</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Trucha entera fresca</t>
+          <t>Sopa de pollo (caja)</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>Uchuva con cáscara</t>
+          <t>Tangelo</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>Ulluco</t>
+          <t>Tilapia roja entera congelada</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>P077</t>
+          <t>E043</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>Uva importada</t>
-        </is>
-      </c>
-      <c r="B352" t="inlineStr">
-        <is>
-          <t>C085</t>
+          <t>Tilapia roja entera fresca</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>Uva Isabela</t>
+          <t>Tilapia, filete congelado</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>C086</t>
+          <t>E030</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>Uva negra</t>
+          <t>Tilapia, lomitos</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>Uva red globe nacional</t>
+          <t>Tomate chonto</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>C085</t>
+          <t>B103</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>Uva roja</t>
+          <t>Tomate chonto regional</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>Uva verde</t>
+          <t>Tomate chonto valluno</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>Vinagre</t>
+          <t>Tomate de árbol</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>C082</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Yuca chirosa</t>
+          <t>Tomate larga vida</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>B103</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>Yuca criolla</t>
+          <t>Tomate riñón</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>Yuca ICA</t>
-        </is>
-      </c>
-      <c r="B361" t="inlineStr">
-        <is>
-          <t>B107</t>
+          <t>Tomate riñón valluno</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>Yuca llanera</t>
+          <t>Tomate Riogrande</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>Zanahoria</t>
-        </is>
-      </c>
-      <c r="B363" t="inlineStr">
-        <is>
-          <t>B110</t>
+          <t>Tomate Riogrande bumangués</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>Zanahoria bogotana</t>
-        </is>
-      </c>
-      <c r="B364" t="inlineStr">
-        <is>
-          <t>B110</t>
+          <t>Tomate Riogrande ocañero</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>Zanahoria larga vida</t>
+          <t>Toyo blanco, filete congelado</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
+          <t>Trucha en corte mariposa</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>E047</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>Trucha entera fresca</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>Uchuva con cáscara</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>Ulluco</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>P077</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>Uva importada</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>C085</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>Uva Isabela</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>C086</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>Uva negra</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>Uva red globe nacional</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>C085</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>Uva roja</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>Uva verde</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>Vinagre</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>Yuca chirosa</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>Yuca criolla</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Yuca ICA</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>B107</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Yuca llanera</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Zanahoria</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>B110</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>Zanahoria bogotana</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>B110</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Zanahoria larga vida</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
           <t>Zapote</t>
         </is>
       </c>
-      <c r="B366" t="inlineStr">
+      <c r="B384" t="inlineStr">
         <is>
           <t>C089</t>
         </is>

</xml_diff>